<commit_message>
added usda thermal curve data
</commit_message>
<xml_diff>
--- a/data/thermal-curve/size.xlsx
+++ b/data/thermal-curve/size.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis.plough/Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/thermal-curve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{004A8222-B2D7-F54F-ADBD-B01D2A80A962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EE442D-F734-7A49-8AC9-858AB9B27269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3FB1A6CC-6B8D-8A4B-B932-80B3BDAF7897}"/>
+    <workbookView xWindow="-33900" yWindow="-380" windowWidth="30240" windowHeight="18880" xr2:uid="{3FB1A6CC-6B8D-8A4B-B932-80B3BDAF7897}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,93 +36,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
   <si>
+    <t>length.mm</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>B05</t>
+  </si>
+  <si>
+    <t>B06</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>B08</t>
+  </si>
+  <si>
+    <t>B09</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
     <t>plate</t>
   </si>
   <si>
     <t>well</t>
   </si>
   <si>
-    <t>length.mm</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>A01</t>
-  </si>
-  <si>
-    <t>A02</t>
-  </si>
-  <si>
-    <t>A03</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
-    <t>A05</t>
-  </si>
-  <si>
-    <t>A06</t>
-  </si>
-  <si>
-    <t>A07</t>
-  </si>
-  <si>
-    <t>A08</t>
-  </si>
-  <si>
-    <t>A09</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>B01</t>
-  </si>
-  <si>
-    <t>B02</t>
-  </si>
-  <si>
-    <t>B03</t>
-  </si>
-  <si>
-    <t>B04</t>
-  </si>
-  <si>
-    <t>B05</t>
-  </si>
-  <si>
-    <t>B06</t>
-  </si>
-  <si>
-    <t>B07</t>
-  </si>
-  <si>
-    <t>B08</t>
-  </si>
-  <si>
-    <t>B09</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>B12</t>
+    <t>plate2</t>
+  </si>
+  <si>
+    <t>plate1</t>
   </si>
 </sst>
 </file>
@@ -502,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE83A52-2E92-8C49-ADC7-6E8DF0861D7F}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,16 +522,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,11 +541,11 @@
       <c r="B2">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
       <c r="E2">
         <v>10.448</v>
@@ -552,11 +558,11 @@
       <c r="B3">
         <v>21</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>8.734</v>
@@ -569,11 +575,11 @@
       <c r="B4">
         <v>21</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="C4" t="s">
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>9.23</v>
@@ -586,11 +592,11 @@
       <c r="B5">
         <v>21</v>
       </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="C5" t="s">
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>10.676</v>
@@ -603,11 +609,11 @@
       <c r="B6">
         <v>21</v>
       </c>
-      <c r="C6">
-        <v>2</v>
+      <c r="C6" t="s">
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>11.721</v>
@@ -620,11 +626,11 @@
       <c r="B7">
         <v>21</v>
       </c>
-      <c r="C7">
-        <v>2</v>
+      <c r="C7" t="s">
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>10.449</v>
@@ -637,11 +643,11 @@
       <c r="B8">
         <v>21</v>
       </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>5.47</v>
@@ -654,11 +660,11 @@
       <c r="B9">
         <v>21</v>
       </c>
-      <c r="C9">
-        <v>2</v>
+      <c r="C9" t="s">
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>11.491</v>
@@ -671,11 +677,11 @@
       <c r="B10">
         <v>21</v>
       </c>
-      <c r="C10">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>10.305999999999999</v>
@@ -688,11 +694,11 @@
       <c r="B11">
         <v>21</v>
       </c>
-      <c r="C11">
-        <v>2</v>
+      <c r="C11" t="s">
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>10.166</v>
@@ -705,11 +711,11 @@
       <c r="B12">
         <v>21</v>
       </c>
-      <c r="C12">
-        <v>2</v>
+      <c r="C12" t="s">
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>10.901999999999999</v>
@@ -722,11 +728,11 @@
       <c r="B13">
         <v>21</v>
       </c>
-      <c r="C13">
-        <v>2</v>
+      <c r="C13" t="s">
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E13">
         <v>8.3219999999999992</v>
@@ -739,11 +745,11 @@
       <c r="B14">
         <v>21</v>
       </c>
-      <c r="C14">
-        <v>2</v>
+      <c r="C14" t="s">
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>10.988</v>
@@ -756,11 +762,11 @@
       <c r="B15">
         <v>21</v>
       </c>
-      <c r="C15">
-        <v>2</v>
+      <c r="C15" t="s">
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>4.9260000000000002</v>
@@ -773,11 +779,11 @@
       <c r="B16">
         <v>21</v>
       </c>
-      <c r="C16">
-        <v>2</v>
+      <c r="C16" t="s">
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E16">
         <v>8.0739999999999998</v>
@@ -790,11 +796,11 @@
       <c r="B17">
         <v>21</v>
       </c>
-      <c r="C17">
-        <v>2</v>
+      <c r="C17" t="s">
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E17">
         <v>9.9849999999999994</v>
@@ -807,11 +813,11 @@
       <c r="B18">
         <v>21</v>
       </c>
-      <c r="C18">
-        <v>2</v>
+      <c r="C18" t="s">
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>5.6479999999999997</v>
@@ -824,11 +830,11 @@
       <c r="B19">
         <v>21</v>
       </c>
-      <c r="C19">
-        <v>2</v>
+      <c r="C19" t="s">
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>6.9640000000000004</v>
@@ -841,11 +847,11 @@
       <c r="B20">
         <v>21</v>
       </c>
-      <c r="C20">
-        <v>2</v>
+      <c r="C20" t="s">
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <v>10.676</v>
@@ -858,11 +864,11 @@
       <c r="B21">
         <v>21</v>
       </c>
-      <c r="C21">
-        <v>2</v>
+      <c r="C21" t="s">
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>12.948</v>
@@ -875,11 +881,11 @@
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>2</v>
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22">
         <v>11.05</v>
@@ -892,11 +898,11 @@
       <c r="B23">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>2</v>
+      <c r="C23" t="s">
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E23">
         <v>14.526</v>
@@ -909,11 +915,11 @@
       <c r="B24">
         <v>21</v>
       </c>
-      <c r="C24">
-        <v>2</v>
+      <c r="C24" t="s">
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E24">
         <v>10.622999999999999</v>
@@ -926,11 +932,11 @@
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25">
-        <v>2</v>
+      <c r="C25" t="s">
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E25">
         <v>12.214</v>
@@ -943,11 +949,11 @@
       <c r="B26">
         <v>37</v>
       </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>6.5730000000000004</v>
@@ -960,11 +966,11 @@
       <c r="B27">
         <v>37</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" t="s">
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <v>7.141</v>
@@ -977,11 +983,11 @@
       <c r="B28">
         <v>37</v>
       </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="C28" t="s">
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>8.9030000000000005</v>
@@ -994,11 +1000,11 @@
       <c r="B29">
         <v>37</v>
       </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>11.9</v>
@@ -1011,11 +1017,11 @@
       <c r="B30">
         <v>37</v>
       </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" t="s">
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E30">
         <v>11.163</v>
@@ -1028,11 +1034,11 @@
       <c r="B31">
         <v>37</v>
       </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="C31" t="s">
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>5.1230000000000002</v>
@@ -1045,11 +1051,11 @@
       <c r="B32">
         <v>37</v>
       </c>
-      <c r="C32">
-        <v>1</v>
+      <c r="C32" t="s">
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>11.595000000000001</v>
@@ -1062,11 +1068,11 @@
       <c r="B33">
         <v>37</v>
       </c>
-      <c r="C33">
-        <v>1</v>
+      <c r="C33" t="s">
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>10.843</v>
@@ -1079,11 +1085,11 @@
       <c r="B34">
         <v>37</v>
       </c>
-      <c r="C34">
-        <v>1</v>
+      <c r="C34" t="s">
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E34">
         <v>10.708</v>
@@ -1096,11 +1102,11 @@
       <c r="B35">
         <v>37</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E35">
         <v>9.484</v>
@@ -1113,11 +1119,11 @@
       <c r="B36">
         <v>37</v>
       </c>
-      <c r="C36">
-        <v>1</v>
+      <c r="C36" t="s">
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E36">
         <v>13.167999999999999</v>
@@ -1130,11 +1136,11 @@
       <c r="B37">
         <v>37</v>
       </c>
-      <c r="C37">
-        <v>1</v>
+      <c r="C37" t="s">
+        <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E37">
         <v>12.085000000000001</v>
@@ -1147,11 +1153,11 @@
       <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38">
-        <v>1</v>
+      <c r="C38" t="s">
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E38">
         <v>13.676</v>
@@ -1164,11 +1170,11 @@
       <c r="B39">
         <v>37</v>
       </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="C39" t="s">
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E39">
         <v>14.702</v>
@@ -1181,11 +1187,11 @@
       <c r="B40">
         <v>37</v>
       </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="C40" t="s">
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E40">
         <v>8.2370000000000001</v>
@@ -1198,11 +1204,11 @@
       <c r="B41">
         <v>37</v>
       </c>
-      <c r="C41">
-        <v>1</v>
+      <c r="C41" t="s">
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E41">
         <v>8.8420000000000005</v>
@@ -1215,11 +1221,11 @@
       <c r="B42">
         <v>37</v>
       </c>
-      <c r="C42">
-        <v>1</v>
+      <c r="C42" t="s">
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E42">
         <v>4.6509999999999998</v>
@@ -1232,11 +1238,11 @@
       <c r="B43">
         <v>37</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E43">
         <v>14.831</v>
@@ -1249,11 +1255,11 @@
       <c r="B44">
         <v>37</v>
       </c>
-      <c r="C44">
-        <v>1</v>
+      <c r="C44" t="s">
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E44">
         <v>6.1609999999999996</v>
@@ -1266,11 +1272,11 @@
       <c r="B45">
         <v>37</v>
       </c>
-      <c r="C45">
-        <v>1</v>
+      <c r="C45" t="s">
+        <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E45">
         <v>8.6880000000000006</v>
@@ -1283,11 +1289,11 @@
       <c r="B46">
         <v>37</v>
       </c>
-      <c r="C46">
-        <v>1</v>
+      <c r="C46" t="s">
+        <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E46">
         <v>8.3859999999999992</v>
@@ -1300,11 +1306,11 @@
       <c r="B47">
         <v>37</v>
       </c>
-      <c r="C47">
-        <v>1</v>
+      <c r="C47" t="s">
+        <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E47">
         <v>14.464</v>
@@ -1317,11 +1323,11 @@
       <c r="B48">
         <v>37</v>
       </c>
-      <c r="C48">
-        <v>1</v>
+      <c r="C48" t="s">
+        <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E48">
         <v>7.4119999999999999</v>
@@ -1334,11 +1340,11 @@
       <c r="B49">
         <v>37</v>
       </c>
-      <c r="C49">
-        <v>1</v>
+      <c r="C49" t="s">
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E49">
         <v>8.6140000000000008</v>
@@ -1351,11 +1357,11 @@
       <c r="B50">
         <v>32</v>
       </c>
-      <c r="C50">
-        <v>1</v>
+      <c r="C50" t="s">
+        <v>30</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E50">
         <v>6.7930000000000001</v>
@@ -1368,11 +1374,11 @@
       <c r="B51">
         <v>32</v>
       </c>
-      <c r="C51">
-        <v>1</v>
+      <c r="C51" t="s">
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E51">
         <v>8.1379999999999999</v>
@@ -1385,11 +1391,11 @@
       <c r="B52">
         <v>32</v>
       </c>
-      <c r="C52">
-        <v>1</v>
+      <c r="C52" t="s">
+        <v>30</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52">
         <v>10.122999999999999</v>
@@ -1402,11 +1408,11 @@
       <c r="B53">
         <v>32</v>
       </c>
-      <c r="C53">
-        <v>1</v>
+      <c r="C53" t="s">
+        <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E53">
         <v>8.5939999999999994</v>
@@ -1419,11 +1425,11 @@
       <c r="B54">
         <v>32</v>
       </c>
-      <c r="C54">
-        <v>1</v>
+      <c r="C54" t="s">
+        <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E54">
         <v>11.523999999999999</v>
@@ -1436,11 +1442,11 @@
       <c r="B55">
         <v>32</v>
       </c>
-      <c r="C55">
-        <v>1</v>
+      <c r="C55" t="s">
+        <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E55">
         <v>12.635</v>
@@ -1453,11 +1459,11 @@
       <c r="B56">
         <v>32</v>
       </c>
-      <c r="C56">
-        <v>1</v>
+      <c r="C56" t="s">
+        <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E56">
         <v>9.4489999999999998</v>
@@ -1470,11 +1476,11 @@
       <c r="B57">
         <v>32</v>
       </c>
-      <c r="C57">
-        <v>1</v>
+      <c r="C57" t="s">
+        <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E57">
         <v>12.928000000000001</v>
@@ -1487,11 +1493,11 @@
       <c r="B58">
         <v>32</v>
       </c>
-      <c r="C58">
-        <v>1</v>
+      <c r="C58" t="s">
+        <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E58">
         <v>13.427</v>
@@ -1504,11 +1510,11 @@
       <c r="B59">
         <v>32</v>
       </c>
-      <c r="C59">
-        <v>1</v>
+      <c r="C59" t="s">
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E59">
         <v>11.303000000000001</v>
@@ -1521,11 +1527,11 @@
       <c r="B60">
         <v>32</v>
       </c>
-      <c r="C60">
-        <v>1</v>
+      <c r="C60" t="s">
+        <v>30</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E60">
         <v>13.978999999999999</v>
@@ -1538,11 +1544,11 @@
       <c r="B61">
         <v>32</v>
       </c>
-      <c r="C61">
-        <v>1</v>
+      <c r="C61" t="s">
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E61">
         <v>9.52</v>
@@ -1555,11 +1561,11 @@
       <c r="B62">
         <v>32</v>
       </c>
-      <c r="C62">
-        <v>1</v>
+      <c r="C62" t="s">
+        <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E62">
         <v>11.15</v>
@@ -1572,11 +1578,11 @@
       <c r="B63">
         <v>32</v>
       </c>
-      <c r="C63">
-        <v>1</v>
+      <c r="C63" t="s">
+        <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E63">
         <v>3.8260000000000001</v>
@@ -1589,11 +1595,11 @@
       <c r="B64">
         <v>32</v>
       </c>
-      <c r="C64">
-        <v>1</v>
+      <c r="C64" t="s">
+        <v>30</v>
       </c>
       <c r="D64" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E64">
         <v>14.116</v>
@@ -1606,11 +1612,11 @@
       <c r="B65">
         <v>32</v>
       </c>
-      <c r="C65">
-        <v>1</v>
+      <c r="C65" t="s">
+        <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E65">
         <v>8.0370000000000008</v>
@@ -1623,11 +1629,11 @@
       <c r="B66">
         <v>32</v>
       </c>
-      <c r="C66">
-        <v>1</v>
+      <c r="C66" t="s">
+        <v>30</v>
       </c>
       <c r="D66" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E66">
         <v>6.3890000000000002</v>
@@ -1640,11 +1646,11 @@
       <c r="B67">
         <v>32</v>
       </c>
-      <c r="C67">
-        <v>1</v>
+      <c r="C67" t="s">
+        <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E67">
         <v>8.0020000000000007</v>
@@ -1657,11 +1663,11 @@
       <c r="B68">
         <v>32</v>
       </c>
-      <c r="C68">
-        <v>1</v>
+      <c r="C68" t="s">
+        <v>30</v>
       </c>
       <c r="D68" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E68">
         <v>8.8949999999999996</v>
@@ -1674,11 +1680,11 @@
       <c r="B69">
         <v>32</v>
       </c>
-      <c r="C69">
-        <v>1</v>
+      <c r="C69" t="s">
+        <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E69">
         <v>10.255000000000001</v>
@@ -1691,11 +1697,11 @@
       <c r="B70">
         <v>32</v>
       </c>
-      <c r="C70">
-        <v>1</v>
+      <c r="C70" t="s">
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E70">
         <v>9.9179999999999993</v>
@@ -1708,11 +1714,11 @@
       <c r="B71">
         <v>32</v>
       </c>
-      <c r="C71">
-        <v>1</v>
+      <c r="C71" t="s">
+        <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E71">
         <v>13.467000000000001</v>
@@ -1725,11 +1731,11 @@
       <c r="B72">
         <v>32</v>
       </c>
-      <c r="C72">
-        <v>1</v>
+      <c r="C72" t="s">
+        <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E72">
         <v>14.843999999999999</v>
@@ -1742,11 +1748,11 @@
       <c r="B73">
         <v>32</v>
       </c>
-      <c r="C73">
-        <v>1</v>
+      <c r="C73" t="s">
+        <v>30</v>
       </c>
       <c r="D73" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E73">
         <v>12.407999999999999</v>
@@ -1759,11 +1765,11 @@
       <c r="B74">
         <v>42</v>
       </c>
-      <c r="C74">
-        <v>1</v>
+      <c r="C74" t="s">
+        <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E74">
         <v>10.045</v>
@@ -1776,11 +1782,11 @@
       <c r="B75">
         <v>42</v>
       </c>
-      <c r="C75">
-        <v>1</v>
+      <c r="C75" t="s">
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E75">
         <v>11.955</v>
@@ -1793,11 +1799,11 @@
       <c r="B76">
         <v>42</v>
       </c>
-      <c r="C76">
-        <v>1</v>
+      <c r="C76" t="s">
+        <v>30</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E76">
         <v>10.819000000000001</v>
@@ -1810,11 +1816,11 @@
       <c r="B77">
         <v>42</v>
       </c>
-      <c r="C77">
-        <v>1</v>
+      <c r="C77" t="s">
+        <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E77">
         <v>14.009</v>
@@ -1827,11 +1833,11 @@
       <c r="B78">
         <v>42</v>
       </c>
-      <c r="C78">
-        <v>1</v>
+      <c r="C78" t="s">
+        <v>30</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E78">
         <v>10.055</v>
@@ -1844,11 +1850,11 @@
       <c r="B79">
         <v>42</v>
       </c>
-      <c r="C79">
-        <v>1</v>
+      <c r="C79" t="s">
+        <v>30</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>7.9749999999999996</v>
@@ -1861,11 +1867,11 @@
       <c r="B80">
         <v>42</v>
       </c>
-      <c r="C80">
-        <v>1</v>
+      <c r="C80" t="s">
+        <v>30</v>
       </c>
       <c r="D80" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E80">
         <v>9.41</v>
@@ -1878,11 +1884,11 @@
       <c r="B81">
         <v>42</v>
       </c>
-      <c r="C81">
-        <v>1</v>
+      <c r="C81" t="s">
+        <v>30</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E81">
         <v>14.811</v>
@@ -1895,11 +1901,11 @@
       <c r="B82">
         <v>42</v>
       </c>
-      <c r="C82">
-        <v>1</v>
+      <c r="C82" t="s">
+        <v>30</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E82">
         <v>13.773</v>
@@ -1912,11 +1918,11 @@
       <c r="B83">
         <v>42</v>
       </c>
-      <c r="C83">
-        <v>1</v>
+      <c r="C83" t="s">
+        <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E83">
         <v>9.8870000000000005</v>
@@ -1929,11 +1935,11 @@
       <c r="B84">
         <v>42</v>
       </c>
-      <c r="C84">
-        <v>1</v>
+      <c r="C84" t="s">
+        <v>30</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E84">
         <v>8.8559999999999999</v>
@@ -1946,11 +1952,11 @@
       <c r="B85">
         <v>42</v>
       </c>
-      <c r="C85">
-        <v>1</v>
+      <c r="C85" t="s">
+        <v>30</v>
       </c>
       <c r="D85" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E85">
         <v>9.5690000000000008</v>
@@ -1963,11 +1969,11 @@
       <c r="B86">
         <v>42</v>
       </c>
-      <c r="C86">
-        <v>1</v>
+      <c r="C86" t="s">
+        <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E86">
         <v>11.679</v>
@@ -1980,11 +1986,11 @@
       <c r="B87">
         <v>42</v>
       </c>
-      <c r="C87">
-        <v>1</v>
+      <c r="C87" t="s">
+        <v>30</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E87">
         <v>14.901</v>
@@ -1997,11 +2003,11 @@
       <c r="B88">
         <v>42</v>
       </c>
-      <c r="C88">
-        <v>1</v>
+      <c r="C88" t="s">
+        <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E88">
         <v>9.7539999999999996</v>
@@ -2014,11 +2020,11 @@
       <c r="B89">
         <v>42</v>
       </c>
-      <c r="C89">
-        <v>1</v>
+      <c r="C89" t="s">
+        <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E89">
         <v>12.704000000000001</v>
@@ -2031,11 +2037,11 @@
       <c r="B90">
         <v>42</v>
       </c>
-      <c r="C90">
-        <v>1</v>
+      <c r="C90" t="s">
+        <v>30</v>
       </c>
       <c r="D90" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E90">
         <v>7.7080000000000002</v>
@@ -2048,11 +2054,11 @@
       <c r="B91">
         <v>42</v>
       </c>
-      <c r="C91">
-        <v>1</v>
+      <c r="C91" t="s">
+        <v>30</v>
       </c>
       <c r="D91" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E91">
         <v>8.1959999999999997</v>
@@ -2065,11 +2071,11 @@
       <c r="B92">
         <v>42</v>
       </c>
-      <c r="C92">
-        <v>1</v>
+      <c r="C92" t="s">
+        <v>30</v>
       </c>
       <c r="D92" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E92">
         <v>17.076000000000001</v>
@@ -2082,11 +2088,11 @@
       <c r="B93">
         <v>42</v>
       </c>
-      <c r="C93">
-        <v>1</v>
+      <c r="C93" t="s">
+        <v>30</v>
       </c>
       <c r="D93" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E93">
         <v>12.798999999999999</v>
@@ -2099,11 +2105,11 @@
       <c r="B94">
         <v>42</v>
       </c>
-      <c r="C94">
-        <v>1</v>
+      <c r="C94" t="s">
+        <v>30</v>
       </c>
       <c r="D94" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E94">
         <v>12.484</v>
@@ -2116,11 +2122,11 @@
       <c r="B95">
         <v>42</v>
       </c>
-      <c r="C95">
-        <v>1</v>
+      <c r="C95" t="s">
+        <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E95">
         <v>11.993</v>
@@ -2133,11 +2139,11 @@
       <c r="B96">
         <v>42</v>
       </c>
-      <c r="C96">
-        <v>1</v>
+      <c r="C96" t="s">
+        <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E96">
         <v>15.186999999999999</v>
@@ -2150,11 +2156,11 @@
       <c r="B97">
         <v>42</v>
       </c>
-      <c r="C97">
-        <v>1</v>
+      <c r="C97" t="s">
+        <v>30</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E97">
         <v>12.337999999999999</v>

</xml_diff>